<commit_message>
redone p,d bite 2 analysis refit and ran through analysis again
</commit_message>
<xml_diff>
--- a/spectroscopic_factors/excel/116Cd_p,d_115Cd_bite_2_spec_factors.xlsx
+++ b/spectroscopic_factors/excel/116Cd_p,d_115Cd_bite_2_spec_factors.xlsx
@@ -380,7 +380,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -444,10 +444,13 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1209.698698115968</v>
+        <v>1209.564221739463</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>0.08234972050040781</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -455,13 +458,13 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>1248</v>
+        <v>1209.564221739463</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D6">
-        <v>0.07455618181384788</v>
+        <v>0.01516576261351482</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -469,13 +472,13 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>1266.835523936558</v>
+        <v>1248</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>0.02164655891887044</v>
+        <v>0.07815507531638952</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -483,13 +486,13 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>1292.576849376487</v>
+        <v>1266.460117430137</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D8">
-        <v>0.0179933537212251</v>
+        <v>0.006382493085096246</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -497,13 +500,13 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>1304.669085796047</v>
+        <v>1292.473979699731</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9">
-        <v>0.01839015653800182</v>
+        <v>0.02049772367939864</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -511,13 +514,13 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>1317.3</v>
+        <v>1304.585912295229</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>0.004773763494720345</v>
+        <v>0.02139510558063962</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -525,13 +528,13 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>1339.858266108656</v>
+        <v>1317.3</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>0.006214847888330158</v>
+        <v>0.004773763494720345</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -539,13 +542,13 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>1358.3</v>
+        <v>1339.018418868032</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12">
-        <v>0.4471185482669841</v>
+        <v>0.007785429305680182</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -553,13 +556,13 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>1452.57432135024</v>
+        <v>1358.3</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D13">
-        <v>0.1853507366472997</v>
+        <v>0.4491463597744076</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -567,13 +570,13 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>1468.83392831836</v>
+        <v>1452.267230934101</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D14">
-        <v>0.08373930918244611</v>
+        <v>0.1853376782608937</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -581,13 +584,13 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>1494.833707949056</v>
+        <v>1468.498351606071</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15">
-        <v>0.190068857153683</v>
+        <v>0.08373005724241933</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -595,13 +598,13 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>1516.019112262857</v>
+        <v>1494.44871075181</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D16">
-        <v>0.008685590664150013</v>
+        <v>0.1900417373909443</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -609,13 +612,13 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>1538.877977992587</v>
+        <v>1515.596556909176</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>0.04824299838127441</v>
+        <v>0.3306340570759647</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -623,13 +626,13 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>1574</v>
+        <v>1515.596556909176</v>
       </c>
       <c r="C18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D18">
-        <v>0.07289689843887331</v>
+        <v>0.03880439038249538</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -637,13 +640,13 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>1597</v>
+        <v>1538.408632604229</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19">
-        <v>0.4215158724959887</v>
+        <v>0.04823577340117313</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -651,10 +654,13 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>1617.510255543843</v>
+        <v>1574</v>
       </c>
       <c r="C20">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>0.07289689843887331</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -662,13 +668,13 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>1623.5303045695</v>
+        <v>1597</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D21">
-        <v>0.00236533398991098</v>
+        <v>0.4214536699028364</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -676,13 +682,13 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>1642.72040757164</v>
+        <v>1616.872511864008</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D22">
-        <v>0.02701614410853748</v>
+        <v>0.1079809019393334</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -690,13 +696,13 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>1733.029906448628</v>
+        <v>1623.064919830593</v>
       </c>
       <c r="C23">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D23">
-        <v>0.04642897863860723</v>
+        <v>0.002364844158558736</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -704,13 +710,13 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>1749.052568744919</v>
+        <v>1642.048348574342</v>
       </c>
       <c r="C24">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>0.05871466720160585</v>
+        <v>0.0270023364094122</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -718,10 +724,13 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>1784.455396813212</v>
+        <v>1732.134406941665</v>
       </c>
       <c r="C25">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>0.04641980476414791</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -729,13 +738,13 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>1790.466639336165</v>
+        <v>1747.835619913894</v>
       </c>
       <c r="C26">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D26">
-        <v>0.08068286417800517</v>
+        <v>0.05870067363643368</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -743,13 +752,13 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>1818</v>
+        <v>1772.725731049579</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D27">
-        <v>0.09458467941825316</v>
+        <v>0.006562677749158311</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -757,10 +766,13 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>1840</v>
+        <v>1785.161835361124</v>
       </c>
       <c r="C28">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>0.03823531669500906</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -768,13 +780,13 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>1847.844461395627</v>
+        <v>1795.477475116088</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29">
-        <v>0.002474606908887055</v>
+        <v>0.01013878774325021</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -782,10 +794,13 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>1865.405783696473</v>
+        <v>1805.922029018604</v>
       </c>
       <c r="C30">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>0.01365473893432243</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -793,13 +808,13 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>1876</v>
+        <v>1818</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
       <c r="D31">
-        <v>0.02797650274726685</v>
+        <v>0.08069046492397715</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -807,13 +822,13 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>1912.863147977638</v>
+        <v>1840</v>
       </c>
       <c r="C32">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D32">
-        <v>0.04029058637520583</v>
+        <v>0.06897927026451577</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -821,13 +836,13 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>1928.384178838498</v>
+        <v>1840</v>
       </c>
       <c r="C33">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D33">
-        <v>0.01184057230579896</v>
+        <v>0.01933433709468267</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -835,13 +850,13 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>1943.649203427909</v>
+        <v>1841.298544231364</v>
       </c>
       <c r="C34">
         <v>2</v>
       </c>
       <c r="D34">
-        <v>0.005408698232667018</v>
+        <v>0.007096152909158444</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -849,13 +864,13 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>1953.892111023081</v>
+        <v>1851.005074483267</v>
       </c>
       <c r="C35">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D35">
-        <v>0.05365244234344334</v>
+        <v>0.005867300457096876</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -863,13 +878,13 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>1968.628892790962</v>
+        <v>1865.530752678807</v>
       </c>
       <c r="C36">
         <v>2</v>
       </c>
       <c r="D36">
-        <v>0.006478832412180363</v>
+        <v>0.05153847163427385</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -877,13 +892,13 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>1995.157326186005</v>
+        <v>1876</v>
       </c>
       <c r="C37">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D37">
-        <v>0.04093996980256261</v>
+        <v>0.04793841377196112</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -891,13 +906,13 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>2048.797067609869</v>
+        <v>1885.117065551615</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D38">
-        <v>0.009895184068082747</v>
+        <v>0.01166998750544201</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -905,13 +920,13 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>2074.264181959651</v>
+        <v>1896.361077451411</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D39">
-        <v>0.0131641830072268</v>
+        <v>0.007999904990412195</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -919,13 +934,13 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>2093.259538687286</v>
+        <v>1911.792281651251</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D40">
-        <v>0.008331462133691377</v>
+        <v>0.01694965968195618</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -933,13 +948,13 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>2113.2</v>
+        <v>1924.67520477692</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D41">
-        <v>0.01749109060776083</v>
+        <v>0.01699344876080397</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -947,13 +962,13 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>2134.380226579768</v>
+        <v>1933.550109340654</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D42">
-        <v>0.006720545737034718</v>
+        <v>0.01755077824842062</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -961,13 +976,195 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>2147.790046147956</v>
+        <v>1944.234562301843</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D43">
-        <v>0.005889769393471447</v>
+        <v>0.01052252851291888</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>1959.440632592807</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44">
+        <v>0.01401285418419295</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>1970.376107067389</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <v>0.01625312779948391</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>1986.766402625133</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <v>0.01049407157396844</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>1995.02814271466</v>
+      </c>
+      <c r="C47">
+        <v>6</v>
+      </c>
+      <c r="D47">
+        <v>0.18322299904006</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>2014.856993695083</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>0.001969364201798255</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>2048.833064430492</v>
+      </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
+      <c r="D49">
+        <v>0.03176164738981578</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>2073.838281975398</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
+      </c>
+      <c r="D50">
+        <v>0.04098796786726889</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>2092.576632909581</v>
+      </c>
+      <c r="C51">
+        <v>2</v>
+      </c>
+      <c r="D51">
+        <v>0.02568909853921173</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>2113.24</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
+      </c>
+      <c r="D52">
+        <v>0.4736005212905512</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>2113.24</v>
+      </c>
+      <c r="C53">
+        <v>3</v>
+      </c>
+      <c r="D53">
+        <v>0.1342078440113726</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>2133.721396755173</v>
+      </c>
+      <c r="C54">
+        <v>2</v>
+      </c>
+      <c r="D54">
+        <v>0.2139754723750275</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>2133.721396755173</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+      <c r="D55">
+        <v>0.06640859596183137</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>2148.119842376009</v>
+      </c>
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="D56">
+        <v>0.01106723146435628</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished (p,d) analysis fixed the l_assignment plotting issue due to changing of how matplotlib ploting works Created a tool for summing spectroscopic factors, then used it.
</commit_message>
<xml_diff>
--- a/spectroscopic_factors/excel/116Cd_p,d_115Cd_bite_2_spec_factors.xlsx
+++ b/spectroscopic_factors/excel/116Cd_p,d_115Cd_bite_2_spec_factors.xlsx
@@ -380,7 +380,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -489,10 +489,10 @@
         <v>1266.460117430137</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>0.006382493085096246</v>
+        <v>0.0008324633664117887</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -713,10 +713,10 @@
         <v>1642.048348574342</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>0.0270023364094122</v>
+        <v>0.005786472390968115</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -727,10 +727,10 @@
         <v>1732.134406941665</v>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>0.04641980476414791</v>
+        <v>0.003175346061097805</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -797,10 +797,10 @@
         <v>1805.922029018604</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D30">
-        <v>0.01365473893432243</v>
+        <v>0.0507632814884952</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -828,7 +828,7 @@
         <v>2</v>
       </c>
       <c r="D32">
-        <v>0.06897927026451577</v>
+        <v>0.04066896040262172</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -836,13 +836,13 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>1840</v>
+        <v>1841.298544231364</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D33">
-        <v>0.01933433709468267</v>
+        <v>0.007096152909158444</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -850,13 +850,13 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>1841.298544231364</v>
+        <v>1851.005074483267</v>
       </c>
       <c r="C34">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D34">
-        <v>0.007096152909158444</v>
+        <v>0.005867300457096876</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -864,13 +864,13 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>1851.005074483267</v>
+        <v>1865.530752678807</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D35">
-        <v>0.005867300457096876</v>
+        <v>0.05153847163427385</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -878,13 +878,13 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>1865.530752678807</v>
+        <v>1876</v>
       </c>
       <c r="C36">
         <v>2</v>
       </c>
       <c r="D36">
-        <v>0.05153847163427385</v>
+        <v>0.04793841377196112</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -892,13 +892,13 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>1876</v>
+        <v>1885.117065551615</v>
       </c>
       <c r="C37">
         <v>2</v>
       </c>
       <c r="D37">
-        <v>0.04793841377196112</v>
+        <v>0.01166998750544201</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -906,13 +906,13 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>1885.117065551615</v>
+        <v>1896.361077451411</v>
       </c>
       <c r="C38">
         <v>2</v>
       </c>
       <c r="D38">
-        <v>0.01166998750544201</v>
+        <v>0.007999904990412195</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -920,13 +920,13 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>1896.361077451411</v>
+        <v>1911.792281651251</v>
       </c>
       <c r="C39">
         <v>2</v>
       </c>
       <c r="D39">
-        <v>0.007999904990412195</v>
+        <v>0.01694965968195618</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -934,13 +934,13 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>1911.792281651251</v>
+        <v>1924.67520477692</v>
       </c>
       <c r="C40">
         <v>2</v>
       </c>
       <c r="D40">
-        <v>0.01694965968195618</v>
+        <v>0.01699344876080397</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -948,13 +948,13 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>1924.67520477692</v>
+        <v>1933.550109340654</v>
       </c>
       <c r="C41">
         <v>2</v>
       </c>
       <c r="D41">
-        <v>0.01699344876080397</v>
+        <v>0.01755077824842062</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -962,13 +962,13 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>1933.550109340654</v>
+        <v>1944.234562301843</v>
       </c>
       <c r="C42">
         <v>2</v>
       </c>
       <c r="D42">
-        <v>0.01755077824842062</v>
+        <v>0.01052252851291888</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -976,13 +976,13 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>1944.234562301843</v>
+        <v>1959.440632592807</v>
       </c>
       <c r="C43">
         <v>2</v>
       </c>
       <c r="D43">
-        <v>0.01052252851291888</v>
+        <v>0.01401285418419295</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -990,13 +990,13 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>1959.440632592807</v>
+        <v>1970.376107067389</v>
       </c>
       <c r="C44">
         <v>2</v>
       </c>
       <c r="D44">
-        <v>0.01401285418419295</v>
+        <v>0.01625312779948391</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1004,13 +1004,13 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>1970.376107067389</v>
+        <v>1986.766402625133</v>
       </c>
       <c r="C45">
         <v>2</v>
       </c>
       <c r="D45">
-        <v>0.01625312779948391</v>
+        <v>0.01049407157396844</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1018,13 +1018,13 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>1986.766402625133</v>
+        <v>1995.02814271466</v>
       </c>
       <c r="C46">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D46">
-        <v>0.01049407157396844</v>
+        <v>0.18322299904006</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1032,13 +1032,13 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>1995.02814271466</v>
+        <v>2014.856993695083</v>
       </c>
       <c r="C47">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D47">
-        <v>0.18322299904006</v>
+        <v>0.001969364201798255</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1046,13 +1046,13 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>2014.856993695083</v>
+        <v>2048.833064430492</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D48">
-        <v>0.001969364201798255</v>
+        <v>0.03176164738981578</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1060,13 +1060,13 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>2048.833064430492</v>
+        <v>2073.838281975398</v>
       </c>
       <c r="C49">
         <v>2</v>
       </c>
       <c r="D49">
-        <v>0.03176164738981578</v>
+        <v>0.04098796786726889</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1074,13 +1074,13 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>2073.838281975398</v>
+        <v>2092.576632909581</v>
       </c>
       <c r="C50">
         <v>2</v>
       </c>
       <c r="D50">
-        <v>0.04098796786726889</v>
+        <v>0.02568909853921173</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1088,13 +1088,13 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>2092.576632909581</v>
+        <v>2113.24</v>
       </c>
       <c r="C51">
         <v>2</v>
       </c>
       <c r="D51">
-        <v>0.02568909853921173</v>
+        <v>0.4736005212905512</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1105,10 +1105,10 @@
         <v>2113.24</v>
       </c>
       <c r="C52">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D52">
-        <v>0.4736005212905512</v>
+        <v>0.1342078440113726</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1116,13 +1116,13 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>2113.24</v>
+        <v>2133.721396755173</v>
       </c>
       <c r="C53">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D53">
-        <v>0.1342078440113726</v>
+        <v>0.2139754723750275</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1133,10 +1133,10 @@
         <v>2133.721396755173</v>
       </c>
       <c r="C54">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D54">
-        <v>0.2139754723750275</v>
+        <v>0.06640859596183137</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1144,26 +1144,12 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>2133.721396755173</v>
+        <v>2148.119842376009</v>
       </c>
       <c r="C55">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D55">
-        <v>0.06640859596183137</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="1">
-        <v>54</v>
-      </c>
-      <c r="B56">
-        <v>2148.119842376009</v>
-      </c>
-      <c r="C56">
-        <v>2</v>
-      </c>
-      <c r="D56">
         <v>0.01106723146435628</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed ptolemywriter to work with d,p (also makes you add the reaction properties from a file bu I can't remember if that was this commit redoing 116Cd bite 1 (d,p) for february usual shuffling round of ptolemy outputs
</commit_message>
<xml_diff>
--- a/spectroscopic_factors/excel/116Cd_p,d_115Cd_bite_2_spec_factors.xlsx
+++ b/spectroscopic_factors/excel/116Cd_p,d_115Cd_bite_2_spec_factors.xlsx
@@ -414,10 +414,10 @@
         <v>4</v>
       </c>
       <c r="D2">
-        <v>0.1490276777973729</v>
+        <v>0.1831305083799375</v>
       </c>
       <c r="E2">
-        <v>0.007251346738462776</v>
+        <v>0.008910712656070784</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -431,10 +431,10 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>0.2937404414934305</v>
+        <v>0.3488840590562667</v>
       </c>
       <c r="E3">
-        <v>0.002862269831848287</v>
+        <v>0.003399601062667641</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -448,10 +448,10 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0.03502302754510135</v>
+        <v>0.03672482619990276</v>
       </c>
       <c r="E4">
-        <v>0.0009639365379385692</v>
+        <v>0.001010775033024846</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -465,7 +465,7 @@
         <v>2</v>
       </c>
       <c r="D5">
-        <v>0.07795795274989076</v>
+        <v>0.3941170235889925</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -482,7 +482,7 @@
         <v>4</v>
       </c>
       <c r="D6">
-        <v>0.01309811992587076</v>
+        <v>0.05723718536433164</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -499,10 +499,10 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <v>0.07815507531638952</v>
+        <v>0.09335552920724868</v>
       </c>
       <c r="E7">
-        <v>0.001450300366695888</v>
+        <v>0.001732370645082966</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -516,10 +516,10 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>0.0008324633664117887</v>
+        <v>0.0008708892800979852</v>
       </c>
       <c r="E8">
-        <v>0.0002601448020036839</v>
+        <v>0.0002721529000306204</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -533,10 +533,10 @@
         <v>2</v>
       </c>
       <c r="D9">
-        <v>0.02049772367939864</v>
+        <v>0.02452402671886105</v>
       </c>
       <c r="E9">
-        <v>0.0008710852028429702</v>
+        <v>0.001042189714480151</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -550,10 +550,10 @@
         <v>2</v>
       </c>
       <c r="D10">
-        <v>0.02139510558063962</v>
+        <v>0.02560799712901147</v>
       </c>
       <c r="E10">
-        <v>0.0009290339588017206</v>
+        <v>0.001111969223992835</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -567,10 +567,10 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>0.004773763494720345</v>
+        <v>0.004987041180272033</v>
       </c>
       <c r="E11">
-        <v>0.000429102336604076</v>
+        <v>0.0004482733645188345</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -584,10 +584,10 @@
         <v>2</v>
       </c>
       <c r="D12">
-        <v>0.007785429305680182</v>
+        <v>0.009329231023706615</v>
       </c>
       <c r="E12">
-        <v>0.0005245502014465371</v>
+        <v>0.0006285652108171123</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -601,10 +601,10 @@
         <v>2</v>
       </c>
       <c r="D13">
-        <v>0.4491463597744076</v>
+        <v>0.5386276983092633</v>
       </c>
       <c r="E13">
-        <v>0.003666727657259063</v>
+        <v>0.004397232740232714</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -618,10 +618,10 @@
         <v>4</v>
       </c>
       <c r="D14">
-        <v>0.08340446253726887</v>
+        <v>0.1029674929485241</v>
       </c>
       <c r="E14">
-        <v>0.00583831237760882</v>
+        <v>0.007207724506396686</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -635,10 +635,10 @@
         <v>4</v>
       </c>
       <c r="D15">
-        <v>0.06808118586513147</v>
+        <v>0.08568951338016828</v>
       </c>
       <c r="E15">
-        <v>0.003275876521375345</v>
+        <v>0.004126522960580352</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -652,10 +652,10 @@
         <v>5</v>
       </c>
       <c r="D16">
-        <v>0.1900417373909443</v>
+        <v>0.211649057127671</v>
       </c>
       <c r="E16">
-        <v>0.01181851600689953</v>
+        <v>0.01316225479649695</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -666,10 +666,10 @@
         <v>1515.596556909176</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D17">
-        <v>0.2269019553533708</v>
+        <v>0.1748704491175608</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -683,10 +683,10 @@
         <v>1515.596556909176</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>0.03534896350903715</v>
+        <v>0.2980911743263773</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -700,13 +700,13 @@
         <v>1538.408632604229</v>
       </c>
       <c r="C19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D19">
-        <v>0.04823577340117313</v>
+        <v>0.009780505139697001</v>
       </c>
       <c r="E19">
-        <v>0.004823577340117314</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -714,16 +714,16 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>1574</v>
+        <v>1538.408632604229</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>0.07289689843887331</v>
+        <v>0.08873337631849795</v>
       </c>
       <c r="E20">
-        <v>0.009183861220645457</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -731,16 +731,16 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>1597</v>
+        <v>1574</v>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D21">
-        <v>0.4214536699028364</v>
+        <v>0.09007138178732341</v>
       </c>
       <c r="E21">
-        <v>0.01760131336021126</v>
+        <v>0.01134757565824547</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -748,16 +748,16 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>1613.149084845743</v>
+        <v>1597</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D22">
-        <v>0.003351768912339795</v>
+        <v>0.4693091437181121</v>
       </c>
       <c r="E22">
-        <v>0.0003511376955784547</v>
+        <v>0.01959991783509517</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -765,16 +765,16 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>1625.344244785309</v>
+        <v>1613.149084845743</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>0.004628586547637729</v>
+        <v>0.003510066718336034</v>
       </c>
       <c r="E23">
-        <v>0.0006612266496625326</v>
+        <v>0.0003677212752542511</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -782,16 +782,16 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>1649.346715797556</v>
+        <v>1625.344244785309</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D24">
-        <v>0.0270023364094122</v>
+        <v>0.00562200978141457</v>
       </c>
       <c r="E24">
-        <v>0.0009915178608107295</v>
+        <v>0.0008031442544877955</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -799,16 +799,16 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>1732.134406941665</v>
+        <v>1649.346715797556</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25">
-        <v>0.003175346061097805</v>
+        <v>0.02792016584155405</v>
       </c>
       <c r="E25">
-        <v>0.0004885147786304314</v>
+        <v>0.001025220287939561</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -816,16 +816,16 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>1747.835619913894</v>
+        <v>1732.134406941665</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D26">
-        <v>0.05870067363643368</v>
+        <v>0.00327370342812974</v>
       </c>
       <c r="E26">
-        <v>0.00571955281585764</v>
+        <v>0.0005036466812507292</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -833,16 +833,16 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>1772.725731049579</v>
+        <v>1747.835619913894</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D27">
-        <v>0.006562677749158311</v>
+        <v>0.07256872219589559</v>
       </c>
       <c r="E27">
-        <v>0.0004732700299873783</v>
+        <v>0.007070798572933417</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -850,16 +850,16 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>1785.161835361124</v>
+        <v>1772.725731049579</v>
       </c>
       <c r="C28">
         <v>2</v>
       </c>
       <c r="D28">
-        <v>0.03823531669500906</v>
+        <v>0.007982132275190436</v>
       </c>
       <c r="E28">
-        <v>0.001203763077390509</v>
+        <v>0.0005756345390762334</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -867,16 +867,16 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>1795.477475116088</v>
+        <v>1785.161835361124</v>
       </c>
       <c r="C29">
         <v>2</v>
       </c>
       <c r="D29">
-        <v>0.01013878774325021</v>
+        <v>0.04652699544045319</v>
       </c>
       <c r="E29">
-        <v>0.0007310097745917075</v>
+        <v>0.001464810129856853</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -884,16 +884,16 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>1805.922029018604</v>
+        <v>1795.477475116088</v>
       </c>
       <c r="C30">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D30">
-        <v>0.0507632814884952</v>
+        <v>0.01233994884654492</v>
       </c>
       <c r="E30">
-        <v>0.004587043507996554</v>
+        <v>0.0008897141801584115</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -901,16 +901,16 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>1818</v>
+        <v>1805.922029018604</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D31">
-        <v>0.08069046492397715</v>
+        <v>0.06276270414327918</v>
       </c>
       <c r="E31">
-        <v>0.002006116531259101</v>
+        <v>0.005671328687645709</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -918,16 +918,16 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>1840</v>
+        <v>1818</v>
       </c>
       <c r="C32">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D32">
-        <v>0.06460444685554217</v>
+        <v>0.08290223255493233</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>0.002061105229266274</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -941,7 +941,7 @@
         <v>0</v>
       </c>
       <c r="D33">
-        <v>0.01312801055132022</v>
+        <v>0.01424385565275013</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -952,13 +952,13 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>1841.298544231364</v>
+        <v>1840</v>
       </c>
       <c r="C34">
         <v>2</v>
       </c>
       <c r="D34">
-        <v>0.002547702085345394</v>
+        <v>0.01315969530077994</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -975,7 +975,7 @@
         <v>0</v>
       </c>
       <c r="D35">
-        <v>0.002652847806461739</v>
+        <v>0.002951086682371595</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -986,16 +986,16 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>1851.005074483267</v>
+        <v>1841.298544231364</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D36">
-        <v>0.005867300457096876</v>
+        <v>0.002755942173064324</v>
       </c>
       <c r="E36">
-        <v>0.0005333909506451705</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1003,16 +1003,16 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>1865.530752678807</v>
+        <v>1851.005074483267</v>
       </c>
       <c r="C37">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D37">
-        <v>0.05153847163427385</v>
+        <v>0.006019806574205516</v>
       </c>
       <c r="E37">
-        <v>0.001688721187764487</v>
+        <v>0.0005472551431095923</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1020,16 +1020,16 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>1876</v>
+        <v>1865.530752678807</v>
       </c>
       <c r="C38">
         <v>2</v>
       </c>
       <c r="D38">
-        <v>0.04793841377196112</v>
+        <v>0.06287310036905422</v>
       </c>
       <c r="E38">
-        <v>0.001727216811634221</v>
+        <v>0.002060114189786275</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1037,16 +1037,16 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>1885.117065551615</v>
+        <v>1876</v>
       </c>
       <c r="C39">
         <v>2</v>
       </c>
       <c r="D39">
-        <v>0.1510466205143166</v>
+        <v>0.058502030323442</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>0.002107822982421772</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1057,13 +1057,13 @@
         <v>1885.117065551615</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D40">
-        <v>0.003039328872354414</v>
+        <v>0.01424527025854633</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <v>0.00163601143025322</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1074,13 +1074,13 @@
         <v>1896.361077451411</v>
       </c>
       <c r="C41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D41">
-        <v>0.007999904990412195</v>
+        <v>0.002012867641817251</v>
       </c>
       <c r="E41">
-        <v>0.000557370429659866</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1088,16 +1088,16 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>1911.792281651251</v>
+        <v>1896.361077451411</v>
       </c>
       <c r="C42">
         <v>2</v>
       </c>
       <c r="D42">
-        <v>0.01694965968195618</v>
+        <v>0.2158831510436833</v>
       </c>
       <c r="E42">
-        <v>0.0009544468558771441</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1105,16 +1105,16 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>1924.67520477692</v>
+        <v>1911.792281651251</v>
       </c>
       <c r="C43">
         <v>2</v>
       </c>
       <c r="D43">
-        <v>0.01699344876080397</v>
+        <v>0.02070507690862477</v>
       </c>
       <c r="E43">
-        <v>0.004760810547773875</v>
+        <v>0.001165916952136152</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1122,16 +1122,16 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>1933.550109340654</v>
+        <v>1924.67520477692</v>
       </c>
       <c r="C44">
         <v>2</v>
       </c>
       <c r="D44">
-        <v>0.01755077824842062</v>
+        <v>0.02076817857046758</v>
       </c>
       <c r="E44">
-        <v>0.004047627497745399</v>
+        <v>0.00581832240106485</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1139,16 +1139,16 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>1944.234562301843</v>
+        <v>1933.550109340654</v>
       </c>
       <c r="C45">
         <v>2</v>
       </c>
       <c r="D45">
-        <v>0.01052252851291888</v>
+        <v>0.02145826195326309</v>
       </c>
       <c r="E45">
-        <v>0.001698256184047034</v>
+        <v>0.004948786310582415</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1156,16 +1156,16 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>1959.440632592807</v>
+        <v>1944.234562301843</v>
       </c>
       <c r="C46">
         <v>2</v>
       </c>
       <c r="D46">
-        <v>0.01401285418419295</v>
+        <v>0.0128703089928519</v>
       </c>
       <c r="E46">
-        <v>0.001137081246450025</v>
+        <v>0.002077170122264074</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1173,16 +1173,16 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>1970.376107067389</v>
+        <v>1959.440632592807</v>
       </c>
       <c r="C47">
         <v>2</v>
       </c>
       <c r="D47">
-        <v>0.01625312779948391</v>
+        <v>0.01714553141885607</v>
       </c>
       <c r="E47">
-        <v>0.001175329489632101</v>
+        <v>0.001391284172413141</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1190,16 +1190,16 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>1986.766402625133</v>
+        <v>1970.376107067389</v>
       </c>
       <c r="C48">
         <v>2</v>
       </c>
       <c r="D48">
-        <v>0.01049407157396844</v>
+        <v>0.01989636215762547</v>
       </c>
       <c r="E48">
-        <v>0.0007760888945378589</v>
+        <v>0.001438786519662999</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1207,16 +1207,16 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>1995.02814271466</v>
+        <v>1986.766402625133</v>
       </c>
       <c r="C49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D49">
-        <v>0.00358591301441812</v>
+        <v>0.01285158537403391</v>
       </c>
       <c r="E49">
-        <v>0.0002098721842821674</v>
+        <v>0.0009504387897195498</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1224,16 +1224,16 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>2014.856993695083</v>
+        <v>1995.02814271466</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50">
-        <v>0.001969364201798255</v>
+        <v>0.003744696920085261</v>
       </c>
       <c r="E50">
-        <v>0.0001188354704612277</v>
+        <v>0.0002130587752902816</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1241,16 +1241,16 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>2048.833064430492</v>
+        <v>2014.856993695083</v>
       </c>
       <c r="C51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D51">
-        <v>0.03176164738981578</v>
+        <v>0.00202594956888477</v>
       </c>
       <c r="E51">
-        <v>0.001065596395112867</v>
+        <v>0.0001199699214421627</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1258,16 +1258,16 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>2073.838281975398</v>
+        <v>2048.833064430492</v>
       </c>
       <c r="C52">
         <v>2</v>
       </c>
       <c r="D52">
-        <v>0.04098796786726889</v>
+        <v>0.03897266962965387</v>
       </c>
       <c r="E52">
-        <v>0.001247309250398715</v>
+        <v>0.00130752463043211</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1275,16 +1275,16 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>2092.576632909581</v>
+        <v>2073.838281975398</v>
       </c>
       <c r="C53">
         <v>2</v>
       </c>
       <c r="D53">
-        <v>0.02568909853921173</v>
+        <v>0.05033354689199342</v>
       </c>
       <c r="E53">
-        <v>0.00101083291402597</v>
+        <v>0.00153170556898712</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1292,16 +1292,16 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>2113.24</v>
+        <v>2092.576632909581</v>
       </c>
       <c r="C54">
         <v>2</v>
       </c>
       <c r="D54">
-        <v>0.5303015044663604</v>
+        <v>0.03156361021997376</v>
       </c>
       <c r="E54">
-        <v>0</v>
+        <v>0.001241987376362604</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1315,7 +1315,7 @@
         <v>0</v>
       </c>
       <c r="D55">
-        <v>0.01248143625838344</v>
+        <v>0.01323984967128855</v>
       </c>
       <c r="E55">
         <v>0</v>
@@ -1326,13 +1326,13 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>2133.721396755173</v>
+        <v>2113.24</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D56">
-        <v>0.005608549416656394</v>
+        <v>0.01161223233179095</v>
       </c>
       <c r="E56">
         <v>0</v>
@@ -1346,13 +1346,13 @@
         <v>2133.721396755173</v>
       </c>
       <c r="C57">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D57">
-        <v>0.2481396455136796</v>
+        <v>0.03558961231351905</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>0.002065468571766731</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1366,10 +1366,10 @@
         <v>2</v>
       </c>
       <c r="D58">
-        <v>0.01106723146435628</v>
+        <v>0.01361943528461127</v>
       </c>
       <c r="E58">
-        <v>0.0007449098101009035</v>
+        <v>0.0009166927595411432</v>
       </c>
     </row>
   </sheetData>

</xml_diff>